<commit_message>
A paper from TUD has been added and assigned to Rui.
</commit_message>
<xml_diff>
--- a/ReadingList141107.xlsx
+++ b/ReadingList141107.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +66,34 @@
   </si>
   <si>
     <t>Alexandre E. Eichenberger, Peng Wu, Kevin O’Brien</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FastLan: Improving Performance of Software Transactional Memory for Low Thread Counts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jons-Tobias Wamhoff, etc.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPoPP 2013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2013.2.23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张睿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TUD的一个做并行的组的成果，关注一下。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,19 +440,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="8" max="8" width="39.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,8 +475,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -464,7 +496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -479,6 +511,32 @@
       </c>
       <c r="G3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>